<commit_message>
Nuevo campo "Supplied" en el BOM. Opción de copiar BOM desde otro SKU. Nuevos campos informativos.
</commit_message>
<xml_diff>
--- a/BOM/Resources/Templates/BOM_Template.xlsx
+++ b/BOM/Resources/Templates/BOM_Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario.ruz\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Supply\BOM\Resources\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8AA7596-A809-409B-9CB8-5EDC9D726D4B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6F93E32-E655-4D35-882D-9DB7741E2966}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9330" xr2:uid="{DCDF11B4-EBCB-43BA-B444-EAA74975973D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Factory</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Component code</t>
+  </si>
+  <si>
+    <t>Supplied</t>
   </si>
 </sst>
 </file>
@@ -421,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77696C12-C511-44B4-90DD-0F955A9F9759}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,7 +446,7 @@
     <col min="13" max="13" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -483,8 +486,11 @@
       <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -499,7 +505,7 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -514,7 +520,7 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>

</xml_diff>